<commit_message>
Forgot to start benchmark 1 year after first data point, leading to erratic initial behaviour for GTAA and Ivy
</commit_message>
<xml_diff>
--- a/Historical Prices/Results/All.xlsx
+++ b/Historical Prices/Results/All.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1614973_ed_ac_uk/Documents/Every Day Files/Documents/Finance/Ivy Portfolio/Historical Prices/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{342D5288-C983-4781-AFE5-901B5FF5FC7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED1C65E0-C867-4B29-9B70-23F4445BC791}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{342D5288-C983-4781-AFE5-901B5FF5FC7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A4DA63F4-0FFE-4F8E-8CC2-7366E046E436}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{9730FFBD-C2B9-4AF0-B37B-8DD90657324D}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="B2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,22 +489,22 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0.84335067321643598</v>
+        <v>0.83810981027487397</v>
       </c>
       <c r="D4">
-        <v>0.84980045237667001</v>
+        <v>0.84502819368090598</v>
       </c>
       <c r="E4">
-        <v>0.91171724573929303</v>
+        <v>0.90925664139523099</v>
       </c>
       <c r="F4">
-        <v>0.976518446912928</v>
+        <v>0.97259780002336405</v>
       </c>
       <c r="G4">
-        <v>1.17664954394468</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1.45177242003471</v>
+        <v>1.1807117147805</v>
+      </c>
+      <c r="H4">
+        <v>1.4851402425376501</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -521,13 +521,13 @@
         <v>0.94670237632769805</v>
       </c>
       <c r="F5">
-        <v>0.98232303679625399</v>
+        <v>0.98232303679625299</v>
       </c>
       <c r="G5">
         <v>1.21860810241466</v>
       </c>
       <c r="H5">
-        <v>1.4162692798921701</v>
+        <v>1.45956731063969</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -549,8 +549,8 @@
       <c r="G6" s="1">
         <v>1.2913066924783301</v>
       </c>
-      <c r="H6">
-        <v>1.3717603449553599</v>
+      <c r="H6" s="1">
+        <v>1.6413053895759999</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -567,13 +567,13 @@
         <v>1.03738950876447</v>
       </c>
       <c r="F7">
-        <v>1.0097627396870199</v>
+        <v>1.0097627396870299</v>
       </c>
       <c r="G7">
         <v>1.1341968158523601</v>
       </c>
       <c r="H7">
-        <v>1.28341416821636</v>
+        <v>1.37289396087158</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -617,22 +617,22 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>-0.25271178828636498</v>
+        <v>-0.25750575545606702</v>
       </c>
       <c r="D11">
-        <v>-0.25271178828636498</v>
+        <v>-0.25750575545606702</v>
       </c>
       <c r="E11">
-        <v>-0.25271178828636498</v>
+        <v>-0.25750575545606702</v>
       </c>
       <c r="F11">
-        <v>-0.25271178828636498</v>
+        <v>-0.25750575545606702</v>
       </c>
       <c r="G11">
-        <v>-0.25271178828636498</v>
+        <v>-0.25750575545606702</v>
       </c>
       <c r="H11">
-        <v>-0.25271178828636498</v>
+        <v>-0.25750575545606702</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -663,22 +663,22 @@
         <v>10</v>
       </c>
       <c r="C13" s="1">
-        <v>-5.6664818092968902E-2</v>
+        <v>-5.6664818092968597E-2</v>
       </c>
       <c r="D13" s="1">
-        <v>-6.6867472204538494E-2</v>
+        <v>-6.6867472204538606E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>-8.3905675960594006E-2</v>
+        <v>-8.3905675960593895E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>-0.11790304738742099</v>
+        <v>-0.11790304738742</v>
       </c>
       <c r="G13">
-        <v>-0.16947038886165999</v>
+        <v>-0.16947038886165799</v>
       </c>
       <c r="H13">
-        <v>-0.178515893009879</v>
+        <v>-0.16947038886165799</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -742,22 +742,22 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>11.921238236941299</v>
+        <v>11.593784730166499</v>
       </c>
       <c r="D18">
-        <v>16.6077525969114</v>
+        <v>16.160156639056499</v>
       </c>
       <c r="E18">
-        <v>20.3441463236041</v>
+        <v>19.678905739952299</v>
       </c>
       <c r="F18">
-        <v>16.032261181819699</v>
+        <v>15.6170046920787</v>
       </c>
       <c r="G18">
-        <v>8.1821266594511801</v>
+        <v>7.9625313937175104</v>
       </c>
       <c r="H18">
-        <v>5.2219852984867101</v>
+        <v>5.51203251413878</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -774,13 +774,13 @@
         <v>18.763202027122201</v>
       </c>
       <c r="F19">
-        <v>14.912112055510599</v>
+        <v>14.912112055510701</v>
       </c>
       <c r="G19">
         <v>7.8089479036607701</v>
       </c>
       <c r="H19">
-        <v>5.5275625977001104</v>
+        <v>5.7903069057172898</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -788,22 +788,22 @@
         <v>10</v>
       </c>
       <c r="C20" s="1">
-        <v>66.184006361043203</v>
+        <v>66.184006361043302</v>
       </c>
       <c r="D20" s="1">
-        <v>75.480591191673099</v>
+        <v>75.4805911916729</v>
       </c>
       <c r="E20" s="1">
-        <v>31.010784506711399</v>
-      </c>
-      <c r="F20">
-        <v>18.5267874334459</v>
+        <v>31.010784506711602</v>
+      </c>
+      <c r="F20" s="2">
+        <v>18.526787433446</v>
       </c>
       <c r="G20">
-        <v>9.9169785230666996</v>
+        <v>9.9169785230665806</v>
       </c>
       <c r="H20">
-        <v>5.9524321087724203</v>
+        <v>6.1661769099967598</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -814,19 +814,19 @@
         <v>27.550206521137302</v>
       </c>
       <c r="D21">
-        <v>36.596582940099701</v>
+        <v>36.596582940099601</v>
       </c>
       <c r="E21">
-        <v>23.236473033335098</v>
+        <v>23.236473033334899</v>
       </c>
       <c r="F21" s="1">
-        <v>23.643242745932501</v>
+        <v>23.643242745932302</v>
       </c>
       <c r="G21" s="1">
         <v>12.7592417972034</v>
       </c>
       <c r="H21" s="1">
-        <v>8.2757207956190193</v>
+        <v>8.6241970819911504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>